<commit_message>
upgrade to version 0.1.0 with new python script
</commit_message>
<xml_diff>
--- a/tests/sample.xlsx
+++ b/tests/sample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2720" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14300" yWindow="6820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="767">
   <si>
     <t>Some text</t>
   </si>
@@ -3129,6 +3129,12 @@
   </si>
   <si>
     <t>1 = Hide formula so that it doesn't appear in the formula bar when the cell is selected (only if the sheet is protected).</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Errors</t>
   </si>
 </sst>
 </file>
@@ -3634,10 +3640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3649,7 +3655,7 @@
     <col min="5" max="5" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -3665,8 +3671,14 @@
       <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3682,8 +3694,12 @@
       <c r="E2" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3699,8 +3715,12 @@
       <c r="E3" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" t="e">
+        <f>something</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3716,8 +3736,12 @@
       <c r="E4" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4" t="e">
+        <f>"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3734,7 +3758,7 @@
         <v>41278</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3751,7 +3775,7 @@
         <v>41279.666666666664</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3768,7 +3792,7 @@
         <v>41275.537743055553</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3785,7 +3809,7 @@
         <v>3.9351851851851852E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3802,7 +3826,7 @@
         <v>41277.156481481485</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3819,7 +3843,7 @@
         <v>41278</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3836,7 +3860,7 @@
         <v>41279.666666666664</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3853,7 +3877,7 @@
         <v>41275.537743055553</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3870,7 +3894,7 @@
         <v>3.9351851851851852E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3887,7 +3911,7 @@
         <v>41277.156481481485</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3904,7 +3928,7 @@
         <v>41278</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4531,7 +4555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added support for booleans, better documentation
</commit_message>
<xml_diff>
--- a/tests/sample.xlsx
+++ b/tests/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14300" yWindow="6820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="57440" yWindow="2840" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="768">
   <si>
     <t>Some text</t>
   </si>
@@ -3135,6 +3135,9 @@
   </si>
   <si>
     <t>Errors</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -3640,10 +3643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3655,7 +3658,7 @@
     <col min="5" max="5" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -3677,8 +3680,11 @@
       <c r="G1" s="2" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3698,8 +3704,12 @@
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3719,8 +3729,12 @@
         <f>something</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3740,8 +3754,12 @@
         <f>"abc"+1</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3757,8 +3775,16 @@
       <c r="E5" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" t="e">
+        <f t="shared" ref="G5:G51" si="0">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3774,8 +3800,16 @@
       <c r="E6" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" t="e">
+        <f t="shared" ref="G6:G51" si="1">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H6" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3791,8 +3825,16 @@
       <c r="E7" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" t="e">
+        <f t="shared" ref="G7:G51" si="2">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3808,8 +3850,16 @@
       <c r="E8" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" t="e">
+        <f t="shared" ref="G8:G51" si="3">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3825,8 +3875,16 @@
       <c r="E9" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" t="e">
+        <f t="shared" ref="G9:G51" si="4">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H9" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3842,8 +3900,16 @@
       <c r="E10" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" t="e">
+        <f t="shared" ref="G10:G51" si="5">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3859,8 +3925,16 @@
       <c r="E11" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" t="e">
+        <f t="shared" ref="G11:G51" si="6">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3876,8 +3950,16 @@
       <c r="E12" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" t="e">
+        <f t="shared" ref="G12:G51" si="7">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H12" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3893,8 +3975,16 @@
       <c r="E13" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="G13" t="e">
+        <f t="shared" ref="G13:G51" si="8">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3910,8 +4000,16 @@
       <c r="E14" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="G14" t="e">
+        <f t="shared" ref="G14:G51" si="9">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3927,8 +4025,16 @@
       <c r="E15" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="G15" t="e">
+        <f t="shared" ref="G15:G51" si="10">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3944,8 +4050,16 @@
       <c r="E16" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16" t="e">
+        <f t="shared" ref="G16:G51" si="11">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H16" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3961,8 +4075,16 @@
       <c r="E17" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" t="e">
+        <f t="shared" ref="G17:G51" si="12">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3978,8 +4100,16 @@
       <c r="E18" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18" t="e">
+        <f t="shared" ref="G18:G51" si="13">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H18" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3995,8 +4125,16 @@
       <c r="E19" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19" t="e">
+        <f t="shared" ref="G19:G51" si="14">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H19" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4012,8 +4150,16 @@
       <c r="E20" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20" t="e">
+        <f t="shared" ref="G20:G51" si="15">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4029,8 +4175,16 @@
       <c r="E21" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21" t="e">
+        <f t="shared" ref="G21:G51" si="16">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H21" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4046,8 +4200,16 @@
       <c r="E22" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22" t="e">
+        <f t="shared" ref="G22:G51" si="17">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H22" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4063,8 +4225,16 @@
       <c r="E23" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="G23" t="e">
+        <f t="shared" ref="G23:G51" si="18">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4080,8 +4250,16 @@
       <c r="E24" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="G24" t="e">
+        <f t="shared" ref="G24:G51" si="19">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H24" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4097,8 +4275,16 @@
       <c r="E25" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="G25" t="e">
+        <f t="shared" ref="G25:G51" si="20">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H25" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4114,8 +4300,16 @@
       <c r="E26" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="G26" t="e">
+        <f t="shared" ref="G26:G51" si="21">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4131,8 +4325,16 @@
       <c r="E27" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="G27" t="e">
+        <f t="shared" ref="G27:G51" si="22">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H27" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4148,8 +4350,16 @@
       <c r="E28" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="G28" t="e">
+        <f t="shared" ref="G28:G51" si="23">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H28" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4165,8 +4375,16 @@
       <c r="E29" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="G29" t="e">
+        <f t="shared" ref="G29:G51" si="24">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4182,8 +4400,16 @@
       <c r="E30" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="G30" t="e">
+        <f t="shared" ref="G30:G51" si="25">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H30" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4199,8 +4425,16 @@
       <c r="E31" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="G31" t="e">
+        <f t="shared" ref="G31:G51" si="26">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H31" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4216,8 +4450,16 @@
       <c r="E32" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="G32" t="e">
+        <f t="shared" ref="G32:G51" si="27">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4233,8 +4475,16 @@
       <c r="E33" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="G33" t="e">
+        <f t="shared" ref="G33:G51" si="28">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H33" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4250,8 +4500,16 @@
       <c r="E34" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="G34" t="e">
+        <f t="shared" ref="G34:G51" si="29">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H34" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4267,8 +4525,16 @@
       <c r="E35" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="G35" t="e">
+        <f t="shared" ref="G35:G51" si="30">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4284,8 +4550,16 @@
       <c r="E36" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="G36" t="e">
+        <f t="shared" ref="G36:G51" si="31">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H36" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4301,8 +4575,16 @@
       <c r="E37" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="G37" t="e">
+        <f t="shared" ref="G37:G51" si="32">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H37" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4318,8 +4600,16 @@
       <c r="E38" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="G38" t="e">
+        <f t="shared" ref="G38:G51" si="33">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4335,8 +4625,16 @@
       <c r="E39" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="G39" t="e">
+        <f t="shared" ref="G39:G51" si="34">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H39" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4352,8 +4650,16 @@
       <c r="E40" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="G40" t="e">
+        <f t="shared" ref="G40:G51" si="35">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H40" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4369,8 +4675,16 @@
       <c r="E41" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="G41" t="e">
+        <f t="shared" ref="G41:G51" si="36">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4386,8 +4700,16 @@
       <c r="E42" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="G42" t="e">
+        <f t="shared" ref="G42:G51" si="37">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H42" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4403,8 +4725,16 @@
       <c r="E43" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="G43" t="e">
+        <f t="shared" ref="G43:G51" si="38">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H43" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4420,8 +4750,16 @@
       <c r="E44" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="G44" t="e">
+        <f t="shared" ref="G44:G51" si="39">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H44" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4437,8 +4775,16 @@
       <c r="E45" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="G45" t="e">
+        <f t="shared" ref="G45:G51" si="40">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H45" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4454,8 +4800,16 @@
       <c r="E46" s="4">
         <v>41279.666666666664</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="G46" t="e">
+        <f t="shared" ref="G46:G51" si="41">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H46" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4471,8 +4825,16 @@
       <c r="E47" s="4">
         <v>41275.537743055553</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="G47" t="e">
+        <f t="shared" ref="G47:G51" si="42">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H47" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4488,8 +4850,16 @@
       <c r="E48" s="4">
         <v>3.9351851851851852E-4</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="G48" t="e">
+        <f t="shared" ref="G48:G51" si="43">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H48" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4505,8 +4875,16 @@
       <c r="E49" s="4">
         <v>41277.156481481485</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="G49" t="e">
+        <f t="shared" ref="G49:G51" si="44">"abc"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H49" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4522,8 +4900,16 @@
       <c r="E50" s="4">
         <v>41278</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="G50" t="e">
+        <f t="shared" ref="G50:G51" si="45">1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H50" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4538,6 +4924,14 @@
       </c>
       <c r="E51" s="4">
         <v>41279.666666666664</v>
+      </c>
+      <c r="G51" t="e">
+        <f t="shared" ref="G51" si="46">something</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H51" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>